<commit_message>
Đang làm dở phần thiều thừa chốt ngày 02/03/2023
</commit_message>
<xml_diff>
--- a/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/Template.xlsx
+++ b/QA_REPORT_MONTHLY/GUI/bin/Debug/CONFIG/Template.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hoai\Hoai_Daotao\vs\QA\PROJECT\QA_REPORT_MONTHLY\GUI\bin\Debug\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA414A-3F1E-4416-92CE-4A6D98D17C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5D0D6-6428-4682-A5C6-1BD6F2236ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CCF5CADB-D592-421D-B75E-E07274F2F514}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CCF5CADB-D592-421D-B75E-E07274F2F514}"/>
   </bookViews>
   <sheets>
     <sheet name="tsb1" sheetId="1" r:id="rId1"/>
     <sheet name="TOSIBA_1" sheetId="2" r:id="rId2"/>
     <sheet name="KYOCERA_1" sheetId="3" r:id="rId3"/>
+    <sheet name="FX_1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="23">
   <si>
     <t>機種
 Model</t>
@@ -123,15 +124,21 @@
     <t>未はんだ/はんだ付け漏れ
 Hàn giả</t>
   </si>
+  <si>
+    <t>逆付
+Ngược hướng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0_ "/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +175,30 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -316,14 +347,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -364,6 +400,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,15 +482,11 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -449,22 +494,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -473,10 +510,63 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="8">
+    <cellStyle name="Comma [0] 2" xfId="7" xr:uid="{CF6761A3-6B5A-4133-A952-872F8BD8F183}"/>
+    <cellStyle name="Comma [0] 3" xfId="4" xr:uid="{AA1BFBA9-3E4D-4EBA-9C37-BFB296C067D9}"/>
+    <cellStyle name="Comma 2" xfId="6" xr:uid="{26129E8D-3F72-4F56-808C-F3CA88710669}"/>
+    <cellStyle name="Comma 3" xfId="3" xr:uid="{AFC9F2AD-A687-4E9E-B332-248FE3E3DFA9}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 30" xfId="5" xr:uid="{1FE7DE71-9701-4647-BAA2-028BA62FB527}"/>
     <cellStyle name="パーセント 2" xfId="2" xr:uid="{F23BC3B4-F901-408D-8EC3-AD02F66D86EC}"/>
     <cellStyle name="常规_10月份第一周品质数据表 2" xfId="1" xr:uid="{6DD67E18-CCBF-46B1-ADC8-AFE1542A5E1A}"/>
   </cellStyles>
@@ -900,7 +990,7 @@
   <dimension ref="A1:W154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -909,51 +999,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="18" t="s">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="15"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="101.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
@@ -993,27 +1083,27 @@
       <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="V2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="30"/>
+      <c r="W2" s="34"/>
     </row>
     <row r="3" spans="1:23" ht="20.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="29">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="33">
         <v>2</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="4">
         <f>SUM(I3:U3)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="35">
         <f t="shared" ref="F3:F34" si="0">E3/C3*1000000</f>
         <v>0</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="4">
         <v>80</v>
       </c>
@@ -1034,21 +1124,21 @@
       <c r="W3" s="7"/>
     </row>
     <row r="4" spans="1:23" ht="20.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="29">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="33">
         <v>4</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E39" si="1">SUM(I4:U4)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="4">
         <v>80</v>
       </c>
@@ -1069,21 +1159,21 @@
       <c r="W4" s="7"/>
     </row>
     <row r="5" spans="1:23" ht="20.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="29">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="33">
         <v>246</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="4">
         <v>80</v>
       </c>
@@ -1104,21 +1194,21 @@
       <c r="W5" s="7"/>
     </row>
     <row r="6" spans="1:23" ht="20.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="29">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="33">
         <v>222</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="4">
         <v>80</v>
       </c>
@@ -1139,21 +1229,21 @@
       <c r="W6" s="7"/>
     </row>
     <row r="7" spans="1:23" ht="20.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="29">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="33">
         <v>437</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="4">
         <v>80</v>
       </c>
@@ -1174,21 +1264,21 @@
       <c r="W7" s="7"/>
     </row>
     <row r="8" spans="1:23" ht="20.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="29">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="33">
         <v>276</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="4">
         <f>SUM(I8:U8)</f>
         <v>1</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="35">
         <f>E8/C8*1000000</f>
         <v>3623.1884057971015</v>
       </c>
-      <c r="G8" s="32"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="4">
         <v>80</v>
       </c>
@@ -1211,21 +1301,21 @@
       <c r="W8" s="7"/>
     </row>
     <row r="9" spans="1:23" ht="20.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="29">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="33">
         <v>380</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="4">
         <v>80</v>
       </c>
@@ -1246,21 +1336,21 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" spans="1:23" ht="20.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="29">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="33">
         <v>1</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="32"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="4">
         <v>80</v>
       </c>
@@ -1281,21 +1371,21 @@
       <c r="W10" s="3"/>
     </row>
     <row r="11" spans="1:23" ht="20.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="29">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="33">
         <v>100</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="4">
         <v>80</v>
       </c>
@@ -1316,21 +1406,21 @@
       <c r="W11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="20.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="29">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="33">
         <v>192</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="4">
         <v>80</v>
       </c>
@@ -1351,21 +1441,21 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" spans="1:23" ht="20.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="29">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="33">
         <v>227</v>
       </c>
-      <c r="D13" s="30"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="36"/>
       <c r="H13" s="4">
         <v>80</v>
       </c>
@@ -1386,21 +1476,21 @@
       <c r="W13" s="3"/>
     </row>
     <row r="14" spans="1:23" ht="20.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="29">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="33">
         <v>439</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="32"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="4">
         <v>80</v>
       </c>
@@ -1421,21 +1511,21 @@
       <c r="W14" s="3"/>
     </row>
     <row r="15" spans="1:23" ht="20.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="29">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="33">
         <v>95</v>
       </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="35">
         <f t="shared" si="0"/>
         <v>10526.315789473683</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="4">
         <v>80</v>
       </c>
@@ -1458,21 +1548,21 @@
       <c r="W15" s="3"/>
     </row>
     <row r="16" spans="1:23" ht="20.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="29">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="33">
         <v>95</v>
       </c>
-      <c r="D16" s="30"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="32"/>
+      <c r="G16" s="36"/>
       <c r="H16" s="4">
         <v>80</v>
       </c>
@@ -1493,21 +1583,21 @@
       <c r="W16" s="3"/>
     </row>
     <row r="17" spans="1:23" ht="20.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="29">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="33">
         <v>120</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="32"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="4">
         <v>80</v>
       </c>
@@ -1528,21 +1618,21 @@
       <c r="W17" s="3"/>
     </row>
     <row r="18" spans="1:23" ht="20.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="29">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="33">
         <v>49</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="36"/>
       <c r="H18" s="4">
         <v>80</v>
       </c>
@@ -1563,21 +1653,21 @@
       <c r="W18" s="3"/>
     </row>
     <row r="19" spans="1:23" ht="20.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="29">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="33">
         <v>36</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="36"/>
       <c r="H19" s="4">
         <v>80</v>
       </c>
@@ -1598,21 +1688,21 @@
       <c r="W19" s="3"/>
     </row>
     <row r="20" spans="1:23" ht="20.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="29">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="33">
         <v>254</v>
       </c>
-      <c r="D20" s="30"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="35">
         <f t="shared" si="0"/>
         <v>3937.0078740157478</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="4">
         <v>80</v>
       </c>
@@ -1635,21 +1725,21 @@
       <c r="W20" s="3"/>
     </row>
     <row r="21" spans="1:23" ht="20.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="29">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="33">
         <v>207</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="32"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="4">
         <v>80</v>
       </c>
@@ -1670,21 +1760,21 @@
       <c r="W21" s="3"/>
     </row>
     <row r="22" spans="1:23" ht="20.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="29">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="33">
         <v>520</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="35">
         <f t="shared" si="0"/>
         <v>5769.2307692307695</v>
       </c>
-      <c r="G22" s="32"/>
+      <c r="G22" s="36"/>
       <c r="H22" s="4">
         <v>80</v>
       </c>
@@ -1707,21 +1797,21 @@
       <c r="W22" s="3"/>
     </row>
     <row r="23" spans="1:23" ht="20.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="29">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="33">
         <v>87</v>
       </c>
-      <c r="D23" s="30"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F23" s="31">
+      <c r="F23" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="4">
         <v>80</v>
       </c>
@@ -1742,21 +1832,21 @@
       <c r="W23" s="3"/>
     </row>
     <row r="24" spans="1:23" ht="20.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="29">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="33">
         <v>50</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="32"/>
+      <c r="G24" s="36"/>
       <c r="H24" s="4">
         <v>80</v>
       </c>
@@ -1777,21 +1867,21 @@
       <c r="W24" s="3"/>
     </row>
     <row r="25" spans="1:23" ht="20.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="29">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="33">
         <v>50</v>
       </c>
-      <c r="D25" s="30"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="32"/>
+      <c r="G25" s="36"/>
       <c r="H25" s="4">
         <v>80</v>
       </c>
@@ -1812,21 +1902,21 @@
       <c r="W25" s="3"/>
     </row>
     <row r="26" spans="1:23" ht="20.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="29">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="33">
         <v>5</v>
       </c>
-      <c r="D26" s="30"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="36"/>
       <c r="H26" s="4">
         <v>80</v>
       </c>
@@ -1847,21 +1937,21 @@
       <c r="W26" s="3"/>
     </row>
     <row r="27" spans="1:23" ht="20.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="29">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="33">
         <v>81</v>
       </c>
-      <c r="D27" s="30"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="32"/>
+      <c r="G27" s="36"/>
       <c r="H27" s="4">
         <v>80</v>
       </c>
@@ -1882,21 +1972,21 @@
       <c r="W27" s="3"/>
     </row>
     <row r="28" spans="1:23" ht="20.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="29">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="33">
         <v>30</v>
       </c>
-      <c r="D28" s="30"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="4">
         <v>80</v>
       </c>
@@ -1917,21 +2007,21 @@
       <c r="W28" s="3"/>
     </row>
     <row r="29" spans="1:23" ht="20.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="29">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="33">
         <v>86</v>
       </c>
-      <c r="D29" s="30"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="4">
         <v>80</v>
       </c>
@@ -1952,21 +2042,21 @@
       <c r="W29" s="3"/>
     </row>
     <row r="30" spans="1:23" ht="20.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="29">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="33">
         <v>120</v>
       </c>
-      <c r="D30" s="30"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="32"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="4">
         <v>80</v>
       </c>
@@ -1987,21 +2077,21 @@
       <c r="W30" s="3"/>
     </row>
     <row r="31" spans="1:23" ht="20.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="29">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="33">
         <v>229</v>
       </c>
-      <c r="D31" s="30"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F31" s="31">
+      <c r="F31" s="35">
         <f>E31/C31*1000000</f>
         <v>13100.436681222707</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="36"/>
       <c r="H31" s="4">
         <v>80</v>
       </c>
@@ -2024,21 +2114,21 @@
       <c r="W31" s="3"/>
     </row>
     <row r="32" spans="1:23" ht="20.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="29">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="33">
         <v>3</v>
       </c>
-      <c r="D32" s="30"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F32" s="31">
+      <c r="F32" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="36"/>
       <c r="H32" s="4">
         <v>80</v>
       </c>
@@ -2059,21 +2149,21 @@
       <c r="W32" s="3"/>
     </row>
     <row r="33" spans="1:23" ht="20.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="29">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="33">
         <v>564</v>
       </c>
-      <c r="D33" s="30"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F33" s="31">
+      <c r="F33" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G33" s="32"/>
+      <c r="G33" s="36"/>
       <c r="H33" s="4">
         <v>80</v>
       </c>
@@ -2094,21 +2184,21 @@
       <c r="W33" s="3"/>
     </row>
     <row r="34" spans="1:23" ht="20.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="29">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="33">
         <v>71</v>
       </c>
-      <c r="D34" s="30"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="36"/>
       <c r="H34" s="4">
         <v>80</v>
       </c>
@@ -2129,21 +2219,21 @@
       <c r="W34" s="3"/>
     </row>
     <row r="35" spans="1:23" ht="20.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="29">
+      <c r="A35" s="18"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="33">
         <v>222</v>
       </c>
-      <c r="D35" s="30"/>
+      <c r="D35" s="34"/>
       <c r="E35" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F35" s="31">
+      <c r="F35" s="35">
         <f>E35/C35*1000000</f>
         <v>0</v>
       </c>
-      <c r="G35" s="32"/>
+      <c r="G35" s="36"/>
       <c r="H35" s="4">
         <v>80</v>
       </c>
@@ -2164,21 +2254,21 @@
       <c r="W35" s="3"/>
     </row>
     <row r="36" spans="1:23" ht="20.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="29">
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="33">
         <v>977</v>
       </c>
-      <c r="D36" s="30"/>
+      <c r="D36" s="34"/>
       <c r="E36" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F36" s="31">
+      <c r="F36" s="35">
         <f t="shared" ref="F36:F39" si="2">E36/C36*1000000</f>
         <v>1023.5414534288639</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="36"/>
       <c r="H36" s="4">
         <v>80</v>
       </c>
@@ -2201,21 +2291,21 @@
       <c r="W36" s="3"/>
     </row>
     <row r="37" spans="1:23" ht="20.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="29">
+      <c r="A37" s="18"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="33">
         <v>18</v>
       </c>
-      <c r="D37" s="30"/>
+      <c r="D37" s="34"/>
       <c r="E37" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F37" s="31">
+      <c r="F37" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G37" s="32"/>
+      <c r="G37" s="36"/>
       <c r="H37" s="4">
         <v>80</v>
       </c>
@@ -2236,21 +2326,21 @@
       <c r="W37" s="3"/>
     </row>
     <row r="38" spans="1:23" ht="20.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="29">
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="33">
         <v>19</v>
       </c>
-      <c r="D38" s="30"/>
+      <c r="D38" s="34"/>
       <c r="E38" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F38" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G38" s="32"/>
+      <c r="G38" s="36"/>
       <c r="H38" s="4">
         <v>80</v>
       </c>
@@ -2271,21 +2361,21 @@
       <c r="W38" s="3"/>
     </row>
     <row r="39" spans="1:23" ht="20.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="29">
+      <c r="A39" s="18"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="33">
         <v>22</v>
       </c>
-      <c r="D39" s="30"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F39" s="31">
+      <c r="F39" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G39" s="32"/>
+      <c r="G39" s="36"/>
       <c r="H39" s="4">
         <v>80</v>
       </c>
@@ -2306,23 +2396,23 @@
       <c r="W39" s="3"/>
     </row>
     <row r="40" spans="1:23" ht="20.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="33">
+      <c r="A40" s="20"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="37">
         <f>SUM(C3:D39
 )</f>
         <v>6536</v>
       </c>
-      <c r="D40" s="34"/>
+      <c r="D40" s="38"/>
       <c r="E40" s="11">
         <f>SUM(E3:E39)</f>
         <v>10</v>
       </c>
-      <c r="F40" s="35">
+      <c r="F40" s="39">
         <f>E40/C40*1000000</f>
         <v>1529.9877600979194</v>
       </c>
-      <c r="G40" s="36"/>
+      <c r="G40" s="40"/>
       <c r="H40" s="12" t="s">
         <v>20</v>
       </c>
@@ -2378,464 +2468,464 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="V40" s="16"/>
-      <c r="W40" s="17"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="21"/>
     </row>
     <row r="41" spans="1:23" ht="20.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="15"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
     </row>
     <row r="42" spans="1:23" ht="20.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="19"/>
     </row>
     <row r="43" spans="1:23" ht="20.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="15"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
     </row>
     <row r="44" spans="1:23" ht="20.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
     </row>
     <row r="45" spans="1:23" ht="20.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
     </row>
     <row r="46" spans="1:23" ht="20.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
     </row>
     <row r="47" spans="1:23" ht="20.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="19"/>
     </row>
     <row r="48" spans="1:23" ht="20.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="19"/>
     </row>
     <row r="49" spans="1:2" ht="20.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="15"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="19"/>
     </row>
     <row r="50" spans="1:2" ht="20.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="19"/>
     </row>
     <row r="51" spans="1:2" ht="20.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="18"/>
+      <c r="B51" s="19"/>
     </row>
     <row r="52" spans="1:2" ht="20.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="15"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="19"/>
     </row>
     <row r="53" spans="1:2" ht="20.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="15"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="19"/>
     </row>
     <row r="54" spans="1:2" ht="20.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="15"/>
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
     </row>
     <row r="55" spans="1:2" ht="20.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="15"/>
+      <c r="A55" s="18"/>
+      <c r="B55" s="19"/>
     </row>
     <row r="56" spans="1:2" ht="20.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="15"/>
+      <c r="A56" s="18"/>
+      <c r="B56" s="19"/>
     </row>
     <row r="57" spans="1:2" ht="20.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="15"/>
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
     </row>
     <row r="58" spans="1:2" ht="20.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="19"/>
     </row>
     <row r="59" spans="1:2" ht="20.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="15"/>
+      <c r="A59" s="18"/>
+      <c r="B59" s="19"/>
     </row>
     <row r="60" spans="1:2" ht="20.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="15"/>
+      <c r="A60" s="18"/>
+      <c r="B60" s="19"/>
     </row>
     <row r="61" spans="1:2" ht="20.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="15"/>
+      <c r="A61" s="18"/>
+      <c r="B61" s="19"/>
     </row>
     <row r="62" spans="1:2" ht="20.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="15"/>
+      <c r="A62" s="18"/>
+      <c r="B62" s="19"/>
     </row>
     <row r="63" spans="1:2" ht="20.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="15"/>
+      <c r="A63" s="18"/>
+      <c r="B63" s="19"/>
     </row>
     <row r="64" spans="1:2" ht="20.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="15"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="19"/>
     </row>
     <row r="65" spans="1:2" ht="20.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="15"/>
+      <c r="A65" s="18"/>
+      <c r="B65" s="19"/>
     </row>
     <row r="66" spans="1:2" ht="20.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="15"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="19"/>
     </row>
     <row r="67" spans="1:2" ht="20.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="15"/>
+      <c r="A67" s="18"/>
+      <c r="B67" s="19"/>
     </row>
     <row r="68" spans="1:2" ht="20.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="15"/>
+      <c r="A68" s="18"/>
+      <c r="B68" s="19"/>
     </row>
     <row r="69" spans="1:2" ht="20.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="15"/>
+      <c r="A69" s="18"/>
+      <c r="B69" s="19"/>
     </row>
     <row r="70" spans="1:2" ht="20.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="15"/>
+      <c r="A70" s="18"/>
+      <c r="B70" s="19"/>
     </row>
     <row r="71" spans="1:2" ht="20.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="15"/>
+      <c r="A71" s="18"/>
+      <c r="B71" s="19"/>
     </row>
     <row r="72" spans="1:2" ht="20.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="15"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="19"/>
     </row>
     <row r="73" spans="1:2" ht="20.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="15"/>
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
     </row>
     <row r="74" spans="1:2" ht="20.25">
-      <c r="A74" s="14"/>
-      <c r="B74" s="15"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="19"/>
     </row>
     <row r="75" spans="1:2" ht="20.25">
-      <c r="A75" s="14"/>
-      <c r="B75" s="15"/>
+      <c r="A75" s="18"/>
+      <c r="B75" s="19"/>
     </row>
     <row r="76" spans="1:2" ht="20.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="15"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="19"/>
     </row>
     <row r="77" spans="1:2" ht="20.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="15"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="19"/>
     </row>
     <row r="78" spans="1:2" ht="20.25">
-      <c r="A78" s="16"/>
-      <c r="B78" s="17"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="21"/>
     </row>
     <row r="79" spans="1:2" ht="20.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="15"/>
+      <c r="A79" s="18"/>
+      <c r="B79" s="19"/>
     </row>
     <row r="80" spans="1:2" ht="20.25">
-      <c r="A80" s="14"/>
-      <c r="B80" s="15"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="19"/>
     </row>
     <row r="81" spans="1:2" ht="20.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="15"/>
+      <c r="A81" s="18"/>
+      <c r="B81" s="19"/>
     </row>
     <row r="82" spans="1:2" ht="20.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="15"/>
+      <c r="A82" s="18"/>
+      <c r="B82" s="19"/>
     </row>
     <row r="83" spans="1:2" ht="20.25">
-      <c r="A83" s="14"/>
-      <c r="B83" s="15"/>
+      <c r="A83" s="18"/>
+      <c r="B83" s="19"/>
     </row>
     <row r="84" spans="1:2" ht="20.25">
-      <c r="A84" s="14"/>
-      <c r="B84" s="15"/>
+      <c r="A84" s="18"/>
+      <c r="B84" s="19"/>
     </row>
     <row r="85" spans="1:2" ht="20.25">
-      <c r="A85" s="14"/>
-      <c r="B85" s="15"/>
+      <c r="A85" s="18"/>
+      <c r="B85" s="19"/>
     </row>
     <row r="86" spans="1:2" ht="20.25">
-      <c r="A86" s="14"/>
-      <c r="B86" s="15"/>
+      <c r="A86" s="18"/>
+      <c r="B86" s="19"/>
     </row>
     <row r="87" spans="1:2" ht="20.25">
-      <c r="A87" s="14"/>
-      <c r="B87" s="15"/>
+      <c r="A87" s="18"/>
+      <c r="B87" s="19"/>
     </row>
     <row r="88" spans="1:2" ht="20.25">
-      <c r="A88" s="14"/>
-      <c r="B88" s="15"/>
+      <c r="A88" s="18"/>
+      <c r="B88" s="19"/>
     </row>
     <row r="89" spans="1:2" ht="20.25">
-      <c r="A89" s="14"/>
-      <c r="B89" s="15"/>
+      <c r="A89" s="18"/>
+      <c r="B89" s="19"/>
     </row>
     <row r="90" spans="1:2" ht="20.25">
-      <c r="A90" s="14"/>
-      <c r="B90" s="15"/>
+      <c r="A90" s="18"/>
+      <c r="B90" s="19"/>
     </row>
     <row r="91" spans="1:2" ht="20.25">
-      <c r="A91" s="14"/>
-      <c r="B91" s="15"/>
+      <c r="A91" s="18"/>
+      <c r="B91" s="19"/>
     </row>
     <row r="92" spans="1:2" ht="20.25">
-      <c r="A92" s="14"/>
-      <c r="B92" s="15"/>
+      <c r="A92" s="18"/>
+      <c r="B92" s="19"/>
     </row>
     <row r="93" spans="1:2" ht="20.25">
-      <c r="A93" s="14"/>
-      <c r="B93" s="15"/>
+      <c r="A93" s="18"/>
+      <c r="B93" s="19"/>
     </row>
     <row r="94" spans="1:2" ht="20.25">
-      <c r="A94" s="14"/>
-      <c r="B94" s="15"/>
+      <c r="A94" s="18"/>
+      <c r="B94" s="19"/>
     </row>
     <row r="95" spans="1:2" ht="20.25">
-      <c r="A95" s="14"/>
-      <c r="B95" s="15"/>
+      <c r="A95" s="18"/>
+      <c r="B95" s="19"/>
     </row>
     <row r="96" spans="1:2" ht="20.25">
-      <c r="A96" s="14"/>
-      <c r="B96" s="15"/>
+      <c r="A96" s="18"/>
+      <c r="B96" s="19"/>
     </row>
     <row r="97" spans="1:2" ht="20.25">
-      <c r="A97" s="14"/>
-      <c r="B97" s="15"/>
+      <c r="A97" s="18"/>
+      <c r="B97" s="19"/>
     </row>
     <row r="98" spans="1:2" ht="20.25">
-      <c r="A98" s="14"/>
-      <c r="B98" s="15"/>
+      <c r="A98" s="18"/>
+      <c r="B98" s="19"/>
     </row>
     <row r="99" spans="1:2" ht="20.25">
-      <c r="A99" s="14"/>
-      <c r="B99" s="15"/>
+      <c r="A99" s="18"/>
+      <c r="B99" s="19"/>
     </row>
     <row r="100" spans="1:2" ht="20.25">
-      <c r="A100" s="14"/>
-      <c r="B100" s="15"/>
+      <c r="A100" s="18"/>
+      <c r="B100" s="19"/>
     </row>
     <row r="101" spans="1:2" ht="20.25">
-      <c r="A101" s="14"/>
-      <c r="B101" s="15"/>
+      <c r="A101" s="18"/>
+      <c r="B101" s="19"/>
     </row>
     <row r="102" spans="1:2" ht="20.25">
-      <c r="A102" s="14"/>
-      <c r="B102" s="15"/>
+      <c r="A102" s="18"/>
+      <c r="B102" s="19"/>
     </row>
     <row r="103" spans="1:2" ht="20.25">
-      <c r="A103" s="14"/>
-      <c r="B103" s="15"/>
+      <c r="A103" s="18"/>
+      <c r="B103" s="19"/>
     </row>
     <row r="104" spans="1:2" ht="20.25">
-      <c r="A104" s="14"/>
-      <c r="B104" s="15"/>
+      <c r="A104" s="18"/>
+      <c r="B104" s="19"/>
     </row>
     <row r="105" spans="1:2" ht="20.25">
-      <c r="A105" s="14"/>
-      <c r="B105" s="15"/>
+      <c r="A105" s="18"/>
+      <c r="B105" s="19"/>
     </row>
     <row r="106" spans="1:2" ht="20.25">
-      <c r="A106" s="14"/>
-      <c r="B106" s="15"/>
+      <c r="A106" s="18"/>
+      <c r="B106" s="19"/>
     </row>
     <row r="107" spans="1:2" ht="20.25">
-      <c r="A107" s="14"/>
-      <c r="B107" s="15"/>
+      <c r="A107" s="18"/>
+      <c r="B107" s="19"/>
     </row>
     <row r="108" spans="1:2" ht="20.25">
-      <c r="A108" s="14"/>
-      <c r="B108" s="15"/>
+      <c r="A108" s="18"/>
+      <c r="B108" s="19"/>
     </row>
     <row r="109" spans="1:2" ht="20.25">
-      <c r="A109" s="14"/>
-      <c r="B109" s="15"/>
+      <c r="A109" s="18"/>
+      <c r="B109" s="19"/>
     </row>
     <row r="110" spans="1:2" ht="20.25">
-      <c r="A110" s="14"/>
-      <c r="B110" s="15"/>
+      <c r="A110" s="18"/>
+      <c r="B110" s="19"/>
     </row>
     <row r="111" spans="1:2" ht="20.25">
-      <c r="A111" s="14"/>
-      <c r="B111" s="15"/>
+      <c r="A111" s="18"/>
+      <c r="B111" s="19"/>
     </row>
     <row r="112" spans="1:2" ht="20.25">
-      <c r="A112" s="14"/>
-      <c r="B112" s="15"/>
+      <c r="A112" s="18"/>
+      <c r="B112" s="19"/>
     </row>
     <row r="113" spans="1:2" ht="20.25">
-      <c r="A113" s="14"/>
-      <c r="B113" s="15"/>
+      <c r="A113" s="18"/>
+      <c r="B113" s="19"/>
     </row>
     <row r="114" spans="1:2" ht="20.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="15"/>
+      <c r="A114" s="18"/>
+      <c r="B114" s="19"/>
     </row>
     <row r="115" spans="1:2" ht="20.25">
-      <c r="A115" s="14"/>
-      <c r="B115" s="15"/>
+      <c r="A115" s="18"/>
+      <c r="B115" s="19"/>
     </row>
     <row r="116" spans="1:2" ht="20.25">
-      <c r="A116" s="16"/>
-      <c r="B116" s="17"/>
+      <c r="A116" s="20"/>
+      <c r="B116" s="21"/>
     </row>
     <row r="117" spans="1:2" ht="20.25">
-      <c r="A117" s="14"/>
-      <c r="B117" s="15"/>
+      <c r="A117" s="18"/>
+      <c r="B117" s="19"/>
     </row>
     <row r="118" spans="1:2" ht="20.25">
-      <c r="A118" s="14"/>
-      <c r="B118" s="15"/>
+      <c r="A118" s="18"/>
+      <c r="B118" s="19"/>
     </row>
     <row r="119" spans="1:2" ht="20.25">
-      <c r="A119" s="14"/>
-      <c r="B119" s="15"/>
+      <c r="A119" s="18"/>
+      <c r="B119" s="19"/>
     </row>
     <row r="120" spans="1:2" ht="20.25">
-      <c r="A120" s="14"/>
-      <c r="B120" s="15"/>
+      <c r="A120" s="18"/>
+      <c r="B120" s="19"/>
     </row>
     <row r="121" spans="1:2" ht="20.25">
-      <c r="A121" s="14"/>
-      <c r="B121" s="15"/>
+      <c r="A121" s="18"/>
+      <c r="B121" s="19"/>
     </row>
     <row r="122" spans="1:2" ht="20.25">
-      <c r="A122" s="14"/>
-      <c r="B122" s="15"/>
+      <c r="A122" s="18"/>
+      <c r="B122" s="19"/>
     </row>
     <row r="123" spans="1:2" ht="20.25">
-      <c r="A123" s="14"/>
-      <c r="B123" s="15"/>
+      <c r="A123" s="18"/>
+      <c r="B123" s="19"/>
     </row>
     <row r="124" spans="1:2" ht="20.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="15"/>
+      <c r="A124" s="18"/>
+      <c r="B124" s="19"/>
     </row>
     <row r="125" spans="1:2" ht="20.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="15"/>
+      <c r="A125" s="18"/>
+      <c r="B125" s="19"/>
     </row>
     <row r="126" spans="1:2" ht="20.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="15"/>
+      <c r="A126" s="18"/>
+      <c r="B126" s="19"/>
     </row>
     <row r="127" spans="1:2" ht="20.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="15"/>
+      <c r="A127" s="18"/>
+      <c r="B127" s="19"/>
     </row>
     <row r="128" spans="1:2" ht="20.25">
-      <c r="A128" s="14"/>
-      <c r="B128" s="15"/>
+      <c r="A128" s="18"/>
+      <c r="B128" s="19"/>
     </row>
     <row r="129" spans="1:2" ht="20.25">
-      <c r="A129" s="14"/>
-      <c r="B129" s="15"/>
+      <c r="A129" s="18"/>
+      <c r="B129" s="19"/>
     </row>
     <row r="130" spans="1:2" ht="20.25">
-      <c r="A130" s="14"/>
-      <c r="B130" s="15"/>
+      <c r="A130" s="18"/>
+      <c r="B130" s="19"/>
     </row>
     <row r="131" spans="1:2" ht="20.25">
-      <c r="A131" s="14"/>
-      <c r="B131" s="15"/>
+      <c r="A131" s="18"/>
+      <c r="B131" s="19"/>
     </row>
     <row r="132" spans="1:2" ht="20.25">
-      <c r="A132" s="14"/>
-      <c r="B132" s="15"/>
+      <c r="A132" s="18"/>
+      <c r="B132" s="19"/>
     </row>
     <row r="133" spans="1:2" ht="20.25">
-      <c r="A133" s="14"/>
-      <c r="B133" s="15"/>
+      <c r="A133" s="18"/>
+      <c r="B133" s="19"/>
     </row>
     <row r="134" spans="1:2" ht="20.25">
-      <c r="A134" s="14"/>
-      <c r="B134" s="15"/>
+      <c r="A134" s="18"/>
+      <c r="B134" s="19"/>
     </row>
     <row r="135" spans="1:2" ht="20.25">
-      <c r="A135" s="14"/>
-      <c r="B135" s="15"/>
+      <c r="A135" s="18"/>
+      <c r="B135" s="19"/>
     </row>
     <row r="136" spans="1:2" ht="20.25">
-      <c r="A136" s="14"/>
-      <c r="B136" s="15"/>
+      <c r="A136" s="18"/>
+      <c r="B136" s="19"/>
     </row>
     <row r="137" spans="1:2" ht="20.25">
-      <c r="A137" s="14"/>
-      <c r="B137" s="15"/>
+      <c r="A137" s="18"/>
+      <c r="B137" s="19"/>
     </row>
     <row r="138" spans="1:2" ht="20.25">
-      <c r="A138" s="14"/>
-      <c r="B138" s="15"/>
+      <c r="A138" s="18"/>
+      <c r="B138" s="19"/>
     </row>
     <row r="139" spans="1:2" ht="20.25">
-      <c r="A139" s="14"/>
-      <c r="B139" s="15"/>
+      <c r="A139" s="18"/>
+      <c r="B139" s="19"/>
     </row>
     <row r="140" spans="1:2" ht="20.25">
-      <c r="A140" s="14"/>
-      <c r="B140" s="15"/>
+      <c r="A140" s="18"/>
+      <c r="B140" s="19"/>
     </row>
     <row r="141" spans="1:2" ht="20.25">
-      <c r="A141" s="14"/>
-      <c r="B141" s="15"/>
+      <c r="A141" s="18"/>
+      <c r="B141" s="19"/>
     </row>
     <row r="142" spans="1:2" ht="20.25">
-      <c r="A142" s="14"/>
-      <c r="B142" s="15"/>
+      <c r="A142" s="18"/>
+      <c r="B142" s="19"/>
     </row>
     <row r="143" spans="1:2" ht="20.25">
-      <c r="A143" s="14"/>
-      <c r="B143" s="15"/>
+      <c r="A143" s="18"/>
+      <c r="B143" s="19"/>
     </row>
     <row r="144" spans="1:2" ht="20.25">
-      <c r="A144" s="14"/>
-      <c r="B144" s="15"/>
+      <c r="A144" s="18"/>
+      <c r="B144" s="19"/>
     </row>
     <row r="145" spans="1:2" ht="20.25">
-      <c r="A145" s="14"/>
-      <c r="B145" s="15"/>
+      <c r="A145" s="18"/>
+      <c r="B145" s="19"/>
     </row>
     <row r="146" spans="1:2" ht="20.25">
-      <c r="A146" s="14"/>
-      <c r="B146" s="15"/>
+      <c r="A146" s="18"/>
+      <c r="B146" s="19"/>
     </row>
     <row r="147" spans="1:2" ht="20.25">
-      <c r="A147" s="14"/>
-      <c r="B147" s="15"/>
+      <c r="A147" s="18"/>
+      <c r="B147" s="19"/>
     </row>
     <row r="148" spans="1:2" ht="20.25">
-      <c r="A148" s="14"/>
-      <c r="B148" s="15"/>
+      <c r="A148" s="18"/>
+      <c r="B148" s="19"/>
     </row>
     <row r="149" spans="1:2" ht="20.25">
-      <c r="A149" s="14"/>
-      <c r="B149" s="15"/>
+      <c r="A149" s="18"/>
+      <c r="B149" s="19"/>
     </row>
     <row r="150" spans="1:2" ht="20.25">
-      <c r="A150" s="14"/>
-      <c r="B150" s="15"/>
+      <c r="A150" s="18"/>
+      <c r="B150" s="19"/>
     </row>
     <row r="151" spans="1:2" ht="20.25">
-      <c r="A151" s="14"/>
-      <c r="B151" s="15"/>
+      <c r="A151" s="18"/>
+      <c r="B151" s="19"/>
     </row>
     <row r="152" spans="1:2" ht="20.25">
-      <c r="A152" s="14"/>
-      <c r="B152" s="15"/>
+      <c r="A152" s="18"/>
+      <c r="B152" s="19"/>
     </row>
     <row r="153" spans="1:2" ht="20.25">
-      <c r="A153" s="14"/>
-      <c r="B153" s="15"/>
+      <c r="A153" s="18"/>
+      <c r="B153" s="19"/>
     </row>
     <row r="154" spans="1:2" ht="20.25">
-      <c r="A154" s="16"/>
-      <c r="B154" s="17"/>
+      <c r="A154" s="20"/>
+      <c r="B154" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="236">
@@ -3125,60 +3215,62 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="20.25"/>
   <cols>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="62"/>
+    <col min="2" max="2" width="40.85546875" style="62" customWidth="1"/>
+    <col min="3" max="23" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="20.25">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="18" t="s">
+    <row r="1" spans="1:23">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="22" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="15"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="101.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3218,10 +3310,10 @@
       <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="V2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="30"/>
+      <c r="W2" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3234,6 +3326,7 @@
     <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3241,100 +3334,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABBC015-6AD3-4607-8895-80BFA3508A8A}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="47" customWidth="1"/>
-    <col min="2" max="5" width="11" style="47" customWidth="1"/>
-    <col min="6" max="20" width="9.140625" style="47"/>
+    <col min="1" max="1" width="40.140625" style="16" customWidth="1"/>
+    <col min="2" max="5" width="11" style="16" customWidth="1"/>
+    <col min="6" max="20" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39" t="s">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="37" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="41"/>
+      <c r="T1" s="45"/>
     </row>
     <row r="2" spans="1:20" ht="162">
-      <c r="A2" s="38"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="44" t="s">
+      <c r="O2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="43" t="s">
+      <c r="P2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="43" t="s">
+      <c r="Q2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="43" t="s">
+      <c r="R2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3354,4 +3447,113 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274060A9-3425-470E-81C1-5868FC4C43B7}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25"/>
+  <cols>
+    <col min="1" max="1" width="49" style="63" customWidth="1"/>
+    <col min="2" max="2" width="25" style="63" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="63" customWidth="1"/>
+    <col min="4" max="5" width="19.5703125" style="63" customWidth="1"/>
+    <col min="6" max="16" width="12" style="63" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" style="63" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="63" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="50"/>
+    </row>
+    <row r="2" spans="1:18" ht="189" customHeight="1">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="Q1:R2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>